<commit_message>
add a dictionary of common substitutes so recipes are not crossed off the list because of minor differences
</commit_message>
<xml_diff>
--- a/Pantry.xlsx
+++ b/Pantry.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chani\PycharmProjects\RecipeWebScraper\venv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chani\PycharmProjects\RecipeWebScraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64012270-4A11-461F-BDAA-E0D193E363E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E090398-977B-4ADF-81A7-73C43DB49A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{CE51DFC5-EC06-46B4-9DE0-033023D0EEBE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Ingredients</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>baking powder</t>
+  </si>
+  <si>
+    <t>pudding mix</t>
+  </si>
+  <si>
+    <t>packets</t>
   </si>
 </sst>
 </file>
@@ -443,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D1E01B-F7C7-49C2-B6F9-7C79E0D68386}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -586,12 +592,38 @@
         <v>11</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010070BEF42AC696304395D2853E525FC9EF" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c139d8d342f882bbeb8e9ea5395bcbb1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e230057f-7a2e-41ec-a188-a75fe992d11a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="db6bd313d52daa5448c9c74323e09968" ns3:_="">
     <xsd:import namespace="e230057f-7a2e-41ec-a188-a75fe992d11a"/>
@@ -737,22 +769,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C85E262-AD67-4DA9-9DD8-9AC4F737F9A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e230057f-7a2e-41ec-a188-a75fe992d11a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A6A5A3-8FCD-433A-BD3D-C5C1B08227D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABEE095-6597-41FA-BA58-B6BC466B4B74}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -768,28 +809,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A6A5A3-8FCD-433A-BD3D-C5C1B08227D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C85E262-AD67-4DA9-9DD8-9AC4F737F9A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e230057f-7a2e-41ec-a188-a75fe992d11a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Basically done level one (if I have time, will add: pdf generator of recipe, substitutes dictionary)
</commit_message>
<xml_diff>
--- a/Pantry.xlsx
+++ b/Pantry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chani\PycharmProjects\RecipeWebScraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E090398-977B-4ADF-81A7-73C43DB49A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF21795-2527-4242-BFAF-4BEE9D97E476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{CE51DFC5-EC06-46B4-9DE0-033023D0EEBE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Ingredients</t>
   </si>
@@ -46,18 +46,9 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Flour</t>
-  </si>
-  <si>
     <t>bag</t>
   </si>
   <si>
-    <t>Sugar</t>
-  </si>
-  <si>
-    <t>Oil</t>
-  </si>
-  <si>
     <t>bottle</t>
   </si>
   <si>
@@ -85,9 +76,6 @@
     <t>chocolate chips</t>
   </si>
   <si>
-    <t>brown sugar</t>
-  </si>
-  <si>
     <t>baking soda</t>
   </si>
   <si>
@@ -98,6 +86,21 @@
   </si>
   <si>
     <t>packets</t>
+  </si>
+  <si>
+    <t>flour</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>vanilla</t>
+  </si>
+  <si>
+    <t>white sugar</t>
+  </si>
+  <si>
+    <t>salt</t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D1E01B-F7C7-49C2-B6F9-7C79E0D68386}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -473,134 +476,145 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -609,21 +623,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010070BEF42AC696304395D2853E525FC9EF" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c139d8d342f882bbeb8e9ea5395bcbb1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e230057f-7a2e-41ec-a188-a75fe992d11a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="db6bd313d52daa5448c9c74323e09968" ns3:_="">
     <xsd:import namespace="e230057f-7a2e-41ec-a188-a75fe992d11a"/>
@@ -769,31 +768,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C85E262-AD67-4DA9-9DD8-9AC4F737F9A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e230057f-7a2e-41ec-a188-a75fe992d11a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A6A5A3-8FCD-433A-BD3D-C5C1B08227D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABEE095-6597-41FA-BA58-B6BC466B4B74}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -809,4 +799,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A6A5A3-8FCD-433A-BD3D-C5C1B08227D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C85E262-AD67-4DA9-9DD8-9AC4F737F9A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e230057f-7a2e-41ec-a188-a75fe992d11a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>